<commit_message>
updated outputs_HGR and rejection_threshold
</commit_message>
<xml_diff>
--- a/outputs_HGR/c__Betaproteobacteria.xlsx
+++ b/outputs_HGR/c__Betaproteobacteria.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F147"/>
+  <dimension ref="A1:F199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,17 +573,17 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT11760.fa</t>
+          <t>even_MAG-GUT11729.fa</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="C6" t="n">
-        <v>2.220446049250264e-14</v>
+        <v>0.06818182</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -599,7 +599,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12028.fa</t>
+          <t>even_MAG-GUT11760.fa</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -625,7 +625,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12217.fa</t>
+          <t>even_MAG-GUT12028.fa</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -651,17 +651,17 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12225.fa</t>
+          <t>even_MAG-GUT12217.fa</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C9" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -677,17 +677,17 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12361.fa</t>
+          <t>even_MAG-GUT12225.fa</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="C10" t="n">
-        <v>2.220446049250264e-14</v>
+        <v>0.06818182</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -703,17 +703,17 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12482.fa</t>
+          <t>even_MAG-GUT12256.fa</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="C11" t="n">
-        <v>2.220446049250264e-14</v>
+        <v>0.06818182</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -729,17 +729,17 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12789.fa</t>
+          <t>even_MAG-GUT12361.fa</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C12" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -755,17 +755,17 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12794.fa</t>
+          <t>even_MAG-GUT12377.fa</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="C13" t="n">
-        <v>2.220446049250264e-14</v>
+        <v>0.06818182</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -781,7 +781,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12944.fa</t>
+          <t>even_MAG-GUT12482.fa</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -807,17 +807,17 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT13480.fa</t>
+          <t>even_MAG-GUT12789.fa</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="C15" t="n">
-        <v>2.220446049250264e-14</v>
+        <v>0.06818182</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -833,7 +833,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT13816.fa</t>
+          <t>even_MAG-GUT12794.fa</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -859,7 +859,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT13955.fa</t>
+          <t>even_MAG-GUT12944.fa</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -885,7 +885,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT14172.fa</t>
+          <t>even_MAG-GUT12991.fa</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -911,7 +911,7 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT14572.fa</t>
+          <t>even_MAG-GUT13170.fa</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -937,7 +937,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT14827.fa</t>
+          <t>even_MAG-GUT13480.fa</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -963,7 +963,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT16149.fa</t>
+          <t>even_MAG-GUT13637.fa</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -989,7 +989,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT16625.fa</t>
+          <t>even_MAG-GUT13816.fa</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1015,7 +1015,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT16715.fa</t>
+          <t>even_MAG-GUT13881.fa</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1041,7 +1041,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT16984.fa</t>
+          <t>even_MAG-GUT13955.fa</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1067,7 +1067,7 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT17598.fa</t>
+          <t>even_MAG-GUT14050.fa</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1093,7 +1093,7 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT18024.fa</t>
+          <t>even_MAG-GUT14125.fa</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1119,7 +1119,7 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT19561.fa</t>
+          <t>even_MAG-GUT14172.fa</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1145,7 +1145,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT19599.fa</t>
+          <t>even_MAG-GUT14250.fa</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1171,7 +1171,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT19853.fa</t>
+          <t>even_MAG-GUT14532.fa</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1197,7 +1197,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT2110.fa</t>
+          <t>even_MAG-GUT14572.fa</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1223,7 +1223,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT21424.fa</t>
+          <t>even_MAG-GUT14827.fa</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1249,7 +1249,7 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT22049.fa</t>
+          <t>even_MAG-GUT15246.fa</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1275,7 +1275,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT22670.fa</t>
+          <t>even_MAG-GUT15625.fa</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1301,7 +1301,7 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT24564.fa</t>
+          <t>even_MAG-GUT16149.fa</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1327,7 +1327,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT24606.fa</t>
+          <t>even_MAG-GUT16156.fa</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1353,7 +1353,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT24616.fa</t>
+          <t>even_MAG-GUT16625.fa</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1379,7 +1379,7 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT24657.fa</t>
+          <t>even_MAG-GUT16715.fa</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1405,7 +1405,7 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT24787.fa</t>
+          <t>even_MAG-GUT16984.fa</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1431,7 +1431,7 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT24840.fa</t>
+          <t>even_MAG-GUT17271.fa</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1457,7 +1457,7 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT24988.fa</t>
+          <t>even_MAG-GUT17598.fa</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1483,7 +1483,7 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT25022.fa</t>
+          <t>even_MAG-GUT1763.fa</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1509,7 +1509,7 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT25055.fa</t>
+          <t>even_MAG-GUT18024.fa</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1535,7 +1535,7 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT25307.fa</t>
+          <t>even_MAG-GUT18195.fa</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1561,7 +1561,7 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT25519.fa</t>
+          <t>even_MAG-GUT18210.fa</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1587,7 +1587,7 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT27032.fa</t>
+          <t>even_MAG-GUT18312.fa</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1613,7 +1613,7 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT27097.fa</t>
+          <t>even_MAG-GUT18361.fa</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1639,17 +1639,17 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT28028.fa</t>
+          <t>even_MAG-GUT18974.fa</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C47" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D47" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1665,17 +1665,17 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT28702.fa</t>
+          <t>even_MAG-GUT19408.fa</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C48" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D48" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1691,7 +1691,7 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT29557.fa</t>
+          <t>even_MAG-GUT19561.fa</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1717,7 +1717,7 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT29963.fa</t>
+          <t>even_MAG-GUT19592.fa</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1743,7 +1743,7 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT30085.fa</t>
+          <t>even_MAG-GUT19599.fa</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1769,7 +1769,7 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT32354.fa</t>
+          <t>even_MAG-GUT19853.fa</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1795,17 +1795,17 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT32803.fa</t>
+          <t>even_MAG-GUT2110.fa</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C53" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D53" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1821,7 +1821,7 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT33566.fa</t>
+          <t>even_MAG-GUT21424.fa</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1847,7 +1847,7 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT33914.fa</t>
+          <t>even_MAG-GUT22049.fa</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1873,7 +1873,7 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT35394.fa</t>
+          <t>even_MAG-GUT22670.fa</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1899,7 +1899,7 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT35641.fa</t>
+          <t>even_MAG-GUT22878.fa</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1925,7 +1925,7 @@
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT35747.fa</t>
+          <t>even_MAG-GUT24564.fa</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1951,7 +1951,7 @@
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT36218.fa</t>
+          <t>even_MAG-GUT24606.fa</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1977,17 +1977,17 @@
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT3631.fa</t>
+          <t>even_MAG-GUT24616.fa</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C60" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D60" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT36683.fa</t>
+          <t>even_MAG-GUT24657.fa</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -2029,7 +2029,7 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT37389.fa</t>
+          <t>even_MAG-GUT24787.fa</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -2055,7 +2055,7 @@
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT37939.fa</t>
+          <t>even_MAG-GUT24840.fa</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -2081,7 +2081,7 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT37961.fa</t>
+          <t>even_MAG-GUT24988.fa</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -2107,7 +2107,7 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT38856.fa</t>
+          <t>even_MAG-GUT25022.fa</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -2133,7 +2133,7 @@
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT39108.fa</t>
+          <t>even_MAG-GUT25055.fa</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -2159,7 +2159,7 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT39136.fa</t>
+          <t>even_MAG-GUT25075.fa</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -2185,7 +2185,7 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT39174.fa</t>
+          <t>even_MAG-GUT25223.fa</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -2211,7 +2211,7 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT3922.fa</t>
+          <t>even_MAG-GUT25263.fa</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -2237,7 +2237,7 @@
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT39460.fa</t>
+          <t>even_MAG-GUT25307.fa</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -2263,7 +2263,7 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT3986.fa</t>
+          <t>even_MAG-GUT27032.fa</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -2289,17 +2289,17 @@
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT399.fa</t>
+          <t>even_MAG-GUT27097.fa</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C72" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D72" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2315,7 +2315,7 @@
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT40499.fa</t>
+          <t>even_MAG-GUT28028.fa</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -2341,7 +2341,7 @@
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT41924.fa</t>
+          <t>even_MAG-GUT28136.fa</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -2367,7 +2367,7 @@
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT42294.fa</t>
+          <t>even_MAG-GUT28702.fa</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -2393,17 +2393,17 @@
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT4260.fa</t>
+          <t>even_MAG-GUT29175.fa</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="C76" t="n">
-        <v>2.220446049250264e-14</v>
+        <v>0.06818182</v>
       </c>
       <c r="D76" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2419,7 +2419,7 @@
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT43146.fa</t>
+          <t>even_MAG-GUT29557.fa</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -2445,7 +2445,7 @@
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT4338.fa</t>
+          <t>even_MAG-GUT29963.fa</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -2471,17 +2471,17 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT44855.fa</t>
+          <t>even_MAG-GUT30085.fa</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C79" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D79" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2497,7 +2497,7 @@
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT46199.fa</t>
+          <t>even_MAG-GUT31546.fa</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -2523,17 +2523,17 @@
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT46826.fa</t>
+          <t>even_MAG-GUT31872.fa</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C81" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D81" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2549,7 +2549,7 @@
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT47180.fa</t>
+          <t>even_MAG-GUT32169.fa</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -2575,7 +2575,7 @@
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT4979.fa</t>
+          <t>even_MAG-GUT32354.fa</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -2601,7 +2601,7 @@
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT5085.fa</t>
+          <t>even_MAG-GUT32469.fa</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -2627,7 +2627,7 @@
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT50906.fa</t>
+          <t>even_MAG-GUT32803.fa</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -2653,17 +2653,17 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT53550.fa</t>
+          <t>even_MAG-GUT33566.fa</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C86" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D86" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2679,7 +2679,7 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT56545.fa</t>
+          <t>even_MAG-GUT33914.fa</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -2705,7 +2705,7 @@
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT56566.fa</t>
+          <t>even_MAG-GUT35394.fa</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -2731,7 +2731,7 @@
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT56852.fa</t>
+          <t>even_MAG-GUT35641.fa</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -2757,7 +2757,7 @@
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT57085.fa</t>
+          <t>even_MAG-GUT36027.fa</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -2783,17 +2783,17 @@
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT57200.fa</t>
+          <t>even_MAG-GUT36148.fa</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C91" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D91" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2809,7 +2809,7 @@
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT58179.fa</t>
+          <t>even_MAG-GUT36218.fa</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -2835,7 +2835,7 @@
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT58607.fa</t>
+          <t>even_MAG-GUT3631.fa</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -2861,7 +2861,7 @@
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT60374.fa</t>
+          <t>even_MAG-GUT36683.fa</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -2887,7 +2887,7 @@
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT61794.fa</t>
+          <t>even_MAG-GUT37389.fa</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -2913,7 +2913,7 @@
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT62134.fa</t>
+          <t>even_MAG-GUT37939.fa</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -2939,7 +2939,7 @@
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT62468.fa</t>
+          <t>even_MAG-GUT37961.fa</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -2965,7 +2965,7 @@
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT6615.fa</t>
+          <t>even_MAG-GUT38016.fa</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -2991,7 +2991,7 @@
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT66915.fa</t>
+          <t>even_MAG-GUT38856.fa</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -3017,7 +3017,7 @@
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT6727.fa</t>
+          <t>even_MAG-GUT38999.fa</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -3043,7 +3043,7 @@
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT6753.fa</t>
+          <t>even_MAG-GUT39108.fa</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -3069,7 +3069,7 @@
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT67531.fa</t>
+          <t>even_MAG-GUT39136.fa</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -3095,17 +3095,17 @@
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT6873.fa</t>
+          <t>even_MAG-GUT39174.fa</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C103" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D103" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3121,7 +3121,7 @@
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT68996.fa</t>
+          <t>even_MAG-GUT3922.fa</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -3147,7 +3147,7 @@
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT69662.fa</t>
+          <t>even_MAG-GUT39245.fa</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -3173,17 +3173,17 @@
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT69729.fa</t>
+          <t>even_MAG-GUT39460.fa</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C106" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D106" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3199,7 +3199,7 @@
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT7016.fa</t>
+          <t>even_MAG-GUT3986.fa</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -3225,17 +3225,17 @@
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT7042.fa</t>
+          <t>even_MAG-GUT399.fa</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="C108" t="n">
-        <v>2.220446049250264e-14</v>
+        <v>0.06818182</v>
       </c>
       <c r="D108" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3251,7 +3251,7 @@
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT72283.fa</t>
+          <t>even_MAG-GUT40105.fa</t>
         </is>
       </c>
       <c r="B109" t="n">
@@ -3277,7 +3277,7 @@
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT7328.fa</t>
+          <t>even_MAG-GUT40305.fa</t>
         </is>
       </c>
       <c r="B110" t="n">
@@ -3303,7 +3303,7 @@
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT73909.fa</t>
+          <t>even_MAG-GUT40499.fa</t>
         </is>
       </c>
       <c r="B111" t="n">
@@ -3329,17 +3329,17 @@
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT73910.fa</t>
+          <t>even_MAG-GUT41924.fa</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C112" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D112" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3355,17 +3355,17 @@
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT73967.fa</t>
+          <t>even_MAG-GUT42294.fa</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="C113" t="n">
-        <v>2.220446049250264e-14</v>
+        <v>0.06818182</v>
       </c>
       <c r="D113" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3381,17 +3381,17 @@
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT74302.fa</t>
+          <t>even_MAG-GUT4260.fa</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C114" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D114" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3407,7 +3407,7 @@
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT74311.fa</t>
+          <t>even_MAG-GUT43146.fa</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -3433,7 +3433,7 @@
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT75471.fa</t>
+          <t>even_MAG-GUT43227.fa</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -3459,7 +3459,7 @@
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT75788.fa</t>
+          <t>even_MAG-GUT43254.fa</t>
         </is>
       </c>
       <c r="B117" t="n">
@@ -3485,7 +3485,7 @@
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT75820.fa</t>
+          <t>even_MAG-GUT4338.fa</t>
         </is>
       </c>
       <c r="B118" t="n">
@@ -3511,17 +3511,17 @@
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT75834.fa</t>
+          <t>even_MAG-GUT44855.fa</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="C119" t="n">
-        <v>2.220446049250264e-14</v>
+        <v>0.06818182</v>
       </c>
       <c r="D119" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3537,7 +3537,7 @@
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT76995.fa</t>
+          <t>even_MAG-GUT45352.fa</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -3563,17 +3563,17 @@
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT77348.fa</t>
+          <t>even_MAG-GUT46199.fa</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C121" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D121" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3589,17 +3589,17 @@
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT77357.fa</t>
+          <t>even_MAG-GUT47180.fa</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C122" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D122" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3615,17 +3615,17 @@
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT77371.fa</t>
+          <t>even_MAG-GUT5085.fa</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C123" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D123" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3641,7 +3641,7 @@
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT77389.fa</t>
+          <t>even_MAG-GUT50906.fa</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -3667,17 +3667,17 @@
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT77563.fa</t>
+          <t>even_MAG-GUT50928.fa</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="C125" t="n">
-        <v>2.220446049250264e-14</v>
+        <v>0.06818182</v>
       </c>
       <c r="D125" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3693,7 +3693,7 @@
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT78371.fa</t>
+          <t>even_MAG-GUT56361.fa</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -3719,17 +3719,17 @@
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT80052.fa</t>
+          <t>even_MAG-GUT56545.fa</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C127" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D127" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3745,7 +3745,7 @@
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT80384.fa</t>
+          <t>even_MAG-GUT56566.fa</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -3771,7 +3771,7 @@
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT80449.fa</t>
+          <t>even_MAG-GUT56852.fa</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -3797,17 +3797,17 @@
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT80561.fa</t>
+          <t>even_MAG-GUT57085.fa</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C130" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D130" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3823,7 +3823,7 @@
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT80720.fa</t>
+          <t>even_MAG-GUT57173.fa</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -3849,17 +3849,17 @@
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT80804.fa</t>
+          <t>even_MAG-GUT57200.fa</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="C132" t="n">
-        <v>2.220446049250264e-14</v>
+        <v>0.06818182</v>
       </c>
       <c r="D132" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3875,7 +3875,7 @@
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT81204.fa</t>
+          <t>even_MAG-GUT57726.fa</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -3901,7 +3901,7 @@
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT81560.fa</t>
+          <t>even_MAG-GUT58179.fa</t>
         </is>
       </c>
       <c r="B134" t="n">
@@ -3927,17 +3927,17 @@
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT81784.fa</t>
+          <t>even_MAG-GUT58214.fa</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C135" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D135" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3953,17 +3953,17 @@
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT82115.fa</t>
+          <t>even_MAG-GUT58607.fa</t>
         </is>
       </c>
       <c r="B136" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="C136" t="n">
-        <v>2.220446049250264e-14</v>
+        <v>0.06818182</v>
       </c>
       <c r="D136" t="n">
-        <v>0.9999999999999778</v>
+        <v>0.9318181800000001</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3979,7 +3979,7 @@
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT82789.fa</t>
+          <t>even_MAG-GUT6030.fa</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -4005,7 +4005,7 @@
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT83592.fa</t>
+          <t>even_MAG-GUT60374.fa</t>
         </is>
       </c>
       <c r="B138" t="n">
@@ -4031,7 +4031,7 @@
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT83946.fa</t>
+          <t>even_MAG-GUT61409.fa</t>
         </is>
       </c>
       <c r="B139" t="n">
@@ -4057,7 +4057,7 @@
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT84859.fa</t>
+          <t>even_MAG-GUT61637.fa</t>
         </is>
       </c>
       <c r="B140" t="n">
@@ -4083,17 +4083,17 @@
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT85462.fa</t>
+          <t>even_MAG-GUT61735.fa</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C141" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D141" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4109,17 +4109,17 @@
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT85601.fa</t>
+          <t>even_MAG-GUT61794.fa</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C142" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D142" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -4135,17 +4135,17 @@
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT85702.fa</t>
+          <t>even_MAG-GUT62134.fa</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C143" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D143" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -4161,17 +4161,17 @@
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT86329.fa</t>
+          <t>even_MAG-GUT62370.fa</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C144" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D144" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -4187,7 +4187,7 @@
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT86514.fa</t>
+          <t>even_MAG-GUT62468.fa</t>
         </is>
       </c>
       <c r="B145" t="n">
@@ -4213,17 +4213,17 @@
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT90614.fa</t>
+          <t>even_MAG-GUT6615.fa</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C146" t="n">
-        <v>0.06818182</v>
+        <v>2.220446049250264e-14</v>
       </c>
       <c r="D146" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4239,24 +4239,1376 @@
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT90671.fa</t>
+          <t>even_MAG-GUT66915.fa</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>0.9318181800000001</v>
+        <v>0.9999999999999778</v>
       </c>
       <c r="C147" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D147" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT6727.fa</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C148" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D148" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT6753.fa</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C149" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D149" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT67531.fa</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C150" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D150" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT6784.fa</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C151" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D151" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT6873.fa</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C152" t="n">
         <v>0.06818182</v>
       </c>
-      <c r="D147" t="n">
-        <v>0.9318181800000001</v>
-      </c>
-      <c r="E147" t="inlineStr">
-        <is>
-          <t>o__Burkholderiales</t>
-        </is>
-      </c>
-      <c r="F147" t="inlineStr">
+      <c r="D152" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT68996.fa</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C153" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D153" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT69662.fa</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C154" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D154" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT69729.fa</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C155" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D155" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT7016.fa</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C156" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D156" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT7042.fa</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C157" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D157" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT72283.fa</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C158" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D158" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT7328.fa</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C159" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D159" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT73909.fa</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C160" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D160" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT73910.fa</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C161" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D161" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT73967.fa</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C162" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D162" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT74302.fa</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C163" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D163" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT74311.fa</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C164" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D164" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT75471.fa</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C165" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D165" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT75788.fa</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C166" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D166" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT75820.fa</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C167" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D167" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT75834.fa</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C168" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D168" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT76995.fa</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C169" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D169" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT77348.fa</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C170" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D170" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT77357.fa</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C171" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D171" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT77371.fa</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C172" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D172" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT77389.fa</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C173" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D173" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT77563.fa</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C174" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D174" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT78371.fa</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C175" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D175" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT80384.fa</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C176" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D176" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT80449.fa</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C177" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D177" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT80561.fa</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C178" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D178" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT80720.fa</t>
+        </is>
+      </c>
+      <c r="B179" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C179" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D179" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT80804.fa</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C180" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D180" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT81029.fa</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C181" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D181" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT81145.fa</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C182" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D182" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT81204.fa</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C183" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D183" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT81432.fa</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C184" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D184" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT81523.fa</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C185" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D185" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT82115.fa</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C186" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D186" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT82789.fa</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C187" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D187" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT83592.fa</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C188" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D188" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT83683.fa</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C189" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D189" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT83946.fa</t>
+        </is>
+      </c>
+      <c r="B190" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C190" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D190" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT84479.fa</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C191" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D191" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT84859.fa</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C192" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D192" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT85462.fa</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C193" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D193" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT85601.fa</t>
+        </is>
+      </c>
+      <c r="B194" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C194" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D194" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT85702.fa</t>
+        </is>
+      </c>
+      <c r="B195" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C195" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D195" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT86329.fa</t>
+        </is>
+      </c>
+      <c r="B196" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C196" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D196" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT86341.fa</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C197" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D197" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT86514.fa</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="C198" t="n">
+        <v>2.220446049250264e-14</v>
+      </c>
+      <c r="D198" t="n">
+        <v>0.9999999999999778</v>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="inlineStr">
+        <is>
+          <t>even_MAG-GUT8790.fa</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="C199" t="n">
+        <v>0.06818182</v>
+      </c>
+      <c r="D199" t="n">
+        <v>0.9318181800000001</v>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>o__Burkholderiales</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
         <is>
           <t>o__Burkholderiales</t>
         </is>

</xml_diff>